<commit_message>
Release-11 LPY Cambios ficheros sql de demografia de paraguay
</commit_message>
<xml_diff>
--- a/org.amerpsoft.com.idempiere.editors-com/documentation/Tables.xlsx
+++ b/org.amerpsoft.com.idempiere.editors-com/documentation/Tables.xlsx
@@ -1129,7 +1129,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1640,7 +1640,7 @@
   <dimension ref="A1:AY9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4972,7 +4972,7 @@
   <dimension ref="A1:AY11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5965,13 +5965,13 @@
   <dimension ref="A1:AY10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="17.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="31.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="199.34"/>
   </cols>

</xml_diff>